<commit_message>
added model selection update with heatmap of gridsearch results
</commit_message>
<xml_diff>
--- a/part2/tables-2/metrics_eval_part-2_scale_alphas.xlsx
+++ b/part2/tables-2/metrics_eval_part-2_scale_alphas.xlsx
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,232 +423,692 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.607394</v>
+        <v>0.742962</v>
       </c>
       <c r="B2">
-        <v>0.140621</v>
+        <v>0.1439</v>
       </c>
       <c r="C2">
-        <v>3.16</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>0.658675</v>
+        <v>0.797783</v>
       </c>
       <c r="E2">
-        <v>0.040476</v>
+        <v>0.025601</v>
       </c>
       <c r="F2">
-        <v>0.813358</v>
+        <v>0.887062</v>
       </c>
       <c r="G2">
-        <v>0.741712</v>
+        <v>0.832049</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.5746790000000001</v>
+        <v>0.699498</v>
       </c>
       <c r="B3">
-        <v>0.64469</v>
+        <v>0.344738</v>
       </c>
       <c r="C3">
-        <v>0.75</v>
+        <v>0.18</v>
       </c>
       <c r="D3">
-        <v>0.744265</v>
+        <v>0.866268</v>
       </c>
       <c r="E3">
-        <v>0.04395</v>
+        <v>0.025522</v>
       </c>
       <c r="F3">
-        <v>0.911739</v>
+        <v>0.911672</v>
       </c>
       <c r="G3">
-        <v>0.842306</v>
+        <v>0.887529</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.384433</v>
+        <v>0.686499</v>
       </c>
       <c r="B4">
-        <v>0.066013</v>
+        <v>0.052083</v>
       </c>
       <c r="C4">
-        <v>13.34</v>
+        <v>3.16</v>
       </c>
       <c r="D4">
-        <v>0.426557</v>
+        <v>0.6783940000000001</v>
       </c>
       <c r="E4">
-        <v>0.029435</v>
+        <v>0.016891</v>
       </c>
       <c r="F4">
-        <v>0.5045460000000001</v>
+        <v>0.753938</v>
       </c>
       <c r="G4">
-        <v>0.480702</v>
+        <v>0.7064049999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.050164</v>
+        <v>0.662398</v>
       </c>
       <c r="B5">
-        <v>0.030403</v>
+        <v>0.05546</v>
       </c>
       <c r="C5">
-        <v>56.23</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.060209</v>
+        <v>0.664911</v>
       </c>
       <c r="E5">
-        <v>0.012631</v>
+        <v>0.016397</v>
       </c>
       <c r="F5">
-        <v>0.125598</v>
+        <v>0.718116</v>
       </c>
       <c r="G5">
-        <v>0.088058</v>
+        <v>0.690716</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>-0.111753</v>
+        <v>0.662347</v>
       </c>
       <c r="B6">
-        <v>0.376219</v>
+        <v>0.055437</v>
       </c>
       <c r="C6">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
       <c r="D6">
-        <v>-0.156187</v>
+        <v>0.664844</v>
       </c>
       <c r="E6">
-        <v>0.160667</v>
+        <v>0.016392</v>
       </c>
       <c r="F6">
-        <v>0.281257</v>
+        <v>0.718052</v>
       </c>
       <c r="G6">
-        <v>0.091005</v>
+        <v>0.690648</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>-0.144412</v>
+        <v>0.662207</v>
       </c>
       <c r="B7">
-        <v>0.417429</v>
+        <v>0.055383</v>
       </c>
       <c r="C7">
         <v>0.04</v>
       </c>
       <c r="D7">
-        <v>-0.192409</v>
+        <v>0.66462</v>
       </c>
       <c r="E7">
-        <v>0.164774</v>
+        <v>0.016395</v>
       </c>
       <c r="F7">
-        <v>0.282623</v>
+        <v>0.717857</v>
       </c>
       <c r="G7">
-        <v>0.054735</v>
+        <v>0.690441</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>-0.149347</v>
+        <v>0.661594</v>
       </c>
       <c r="B8">
-        <v>0.422119</v>
+        <v>0.054995</v>
       </c>
       <c r="C8">
-        <v>0.01</v>
+        <v>0.18</v>
       </c>
       <c r="D8">
-        <v>-0.198428</v>
+        <v>0.663781</v>
       </c>
       <c r="E8">
-        <v>0.166111</v>
+        <v>0.016291</v>
       </c>
       <c r="F8">
-        <v>0.282482</v>
+        <v>0.71688</v>
       </c>
       <c r="G8">
-        <v>0.051635</v>
+        <v>0.689415</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>-0.151002</v>
+        <v>0.6604449999999999</v>
       </c>
       <c r="B9">
-        <v>0.423691</v>
+        <v>0.050108</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D9">
-        <v>-0.200446</v>
+        <v>0.659649</v>
       </c>
       <c r="E9">
-        <v>0.166559</v>
+        <v>0.015332</v>
       </c>
       <c r="F9">
-        <v>0.282435</v>
+        <v>0.712843</v>
       </c>
       <c r="G9">
-        <v>0.050596</v>
+        <v>0.683364</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>-0.161926</v>
+        <v>0.620122</v>
       </c>
       <c r="B10">
-        <v>0.031279</v>
+        <v>0.03802</v>
       </c>
       <c r="C10">
-        <v>237.14</v>
+        <v>0.75</v>
       </c>
       <c r="D10">
-        <v>-0.154318</v>
+        <v>0.6238899999999999</v>
       </c>
       <c r="E10">
-        <v>0.005138</v>
+        <v>0.022767</v>
       </c>
       <c r="F10">
-        <v>-0.094455</v>
+        <v>0.692733</v>
       </c>
       <c r="G10">
-        <v>-0.14767</v>
+        <v>0.665485</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>-0.161946</v>
+        <v>0.61006</v>
       </c>
       <c r="B11">
-        <v>0.031269</v>
+        <v>0.040604</v>
       </c>
       <c r="C11">
+        <v>0.18</v>
+      </c>
+      <c r="D11">
+        <v>0.615913</v>
+      </c>
+      <c r="E11">
+        <v>0.018372</v>
+      </c>
+      <c r="F11">
+        <v>0.6810580000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.650166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>0.607384</v>
+      </c>
+      <c r="B12">
+        <v>0.042034</v>
+      </c>
+      <c r="C12">
+        <v>0.04</v>
+      </c>
+      <c r="D12">
+        <v>0.613066</v>
+      </c>
+      <c r="E12">
+        <v>0.019266</v>
+      </c>
+      <c r="F12">
+        <v>0.676463</v>
+      </c>
+      <c r="G12">
+        <v>0.649589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>0.607378</v>
+      </c>
+      <c r="B13">
+        <v>0.041561</v>
+      </c>
+      <c r="C13">
+        <v>0.01</v>
+      </c>
+      <c r="D13">
+        <v>0.61309</v>
+      </c>
+      <c r="E13">
+        <v>0.018756</v>
+      </c>
+      <c r="F13">
+        <v>0.676619</v>
+      </c>
+      <c r="G13">
+        <v>0.649454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>0.607214</v>
+      </c>
+      <c r="B14">
+        <v>0.041586</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.612933</v>
+      </c>
+      <c r="E14">
+        <v>0.018774</v>
+      </c>
+      <c r="F14">
+        <v>0.676636</v>
+      </c>
+      <c r="G14">
+        <v>0.649388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>0.450873</v>
+      </c>
+      <c r="B15">
+        <v>0.055976</v>
+      </c>
+      <c r="C15">
+        <v>13.34</v>
+      </c>
+      <c r="D15">
+        <v>0.446009</v>
+      </c>
+      <c r="E15">
+        <v>0.018852</v>
+      </c>
+      <c r="F15">
+        <v>0.535879</v>
+      </c>
+      <c r="G15">
+        <v>0.481706</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>0.443861</v>
+      </c>
+      <c r="B16">
+        <v>0.036667</v>
+      </c>
+      <c r="C16">
+        <v>3.16</v>
+      </c>
+      <c r="D16">
+        <v>0.442942</v>
+      </c>
+      <c r="E16">
+        <v>0.011889</v>
+      </c>
+      <c r="F16">
+        <v>0.515871</v>
+      </c>
+      <c r="G16">
+        <v>0.465022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>0.268663</v>
+      </c>
+      <c r="B17">
+        <v>0.043651</v>
+      </c>
+      <c r="C17">
+        <v>3.16</v>
+      </c>
+      <c r="D17">
+        <v>0.268018</v>
+      </c>
+      <c r="E17">
+        <v>0.014915</v>
+      </c>
+      <c r="F17">
+        <v>0.371605</v>
+      </c>
+      <c r="G17">
+        <v>0.292417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>0.062761</v>
+      </c>
+      <c r="B18">
+        <v>0.031046</v>
+      </c>
+      <c r="C18">
+        <v>56.23</v>
+      </c>
+      <c r="D18">
+        <v>0.06454500000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.00876</v>
+      </c>
+      <c r="F18">
+        <v>0.106323</v>
+      </c>
+      <c r="G18">
+        <v>0.078473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>0.03495</v>
+      </c>
+      <c r="B19">
+        <v>0.030463</v>
+      </c>
+      <c r="C19">
+        <v>13.34</v>
+      </c>
+      <c r="D19">
+        <v>0.036764</v>
+      </c>
+      <c r="E19">
+        <v>0.007225</v>
+      </c>
+      <c r="F19">
+        <v>0.079619</v>
+      </c>
+      <c r="G19">
+        <v>0.047153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>0.012341</v>
+      </c>
+      <c r="B20">
+        <v>0.030824</v>
+      </c>
+      <c r="C20">
+        <v>13.34</v>
+      </c>
+      <c r="D20">
+        <v>0.014908</v>
+      </c>
+      <c r="E20">
+        <v>0.007852</v>
+      </c>
+      <c r="F20">
+        <v>0.057932</v>
+      </c>
+      <c r="G20">
+        <v>0.028011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>-0.177212</v>
+      </c>
+      <c r="B21">
+        <v>0.029269</v>
+      </c>
+      <c r="C21">
+        <v>56.23</v>
+      </c>
+      <c r="D21">
+        <v>-0.172182</v>
+      </c>
+      <c r="E21">
+        <v>0.004889</v>
+      </c>
+      <c r="F21">
+        <v>-0.143424</v>
+      </c>
+      <c r="G21">
+        <v>-0.160612</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>-0.178526</v>
+      </c>
+      <c r="B22">
+        <v>0.028818</v>
+      </c>
+      <c r="C22">
+        <v>237.14</v>
+      </c>
+      <c r="D22">
+        <v>-0.173397</v>
+      </c>
+      <c r="E22">
+        <v>0.004824</v>
+      </c>
+      <c r="F22">
+        <v>-0.145529</v>
+      </c>
+      <c r="G22">
+        <v>-0.162355</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>-0.178575</v>
+      </c>
+      <c r="B23">
+        <v>0.02883</v>
+      </c>
+      <c r="C23">
         <v>1000</v>
       </c>
-      <c r="D11">
-        <v>-0.154336</v>
-      </c>
-      <c r="E11">
-        <v>0.005154</v>
-      </c>
-      <c r="F11">
-        <v>-0.094487</v>
-      </c>
-      <c r="G11">
-        <v>-0.147669</v>
+      <c r="D23">
+        <v>-0.173444</v>
+      </c>
+      <c r="E23">
+        <v>0.004817</v>
+      </c>
+      <c r="F23">
+        <v>-0.145539</v>
+      </c>
+      <c r="G23">
+        <v>-0.16244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>-0.188545</v>
+      </c>
+      <c r="B24">
+        <v>0.029715</v>
+      </c>
+      <c r="C24">
+        <v>56.23</v>
+      </c>
+      <c r="D24">
+        <v>-0.183435</v>
+      </c>
+      <c r="E24">
+        <v>0.005565</v>
+      </c>
+      <c r="F24">
+        <v>-0.154946</v>
+      </c>
+      <c r="G24">
+        <v>-0.17233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>-0.19637</v>
+      </c>
+      <c r="B25">
+        <v>0.029806</v>
+      </c>
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="D25">
+        <v>-0.191095</v>
+      </c>
+      <c r="E25">
+        <v>0.005582</v>
+      </c>
+      <c r="F25">
+        <v>-0.162908</v>
+      </c>
+      <c r="G25">
+        <v>-0.177966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>-0.202867</v>
+      </c>
+      <c r="B26">
+        <v>0.030503</v>
+      </c>
+      <c r="C26">
+        <v>1000</v>
+      </c>
+      <c r="D26">
+        <v>-0.197544</v>
+      </c>
+      <c r="E26">
+        <v>0.005625</v>
+      </c>
+      <c r="F26">
+        <v>-0.168233</v>
+      </c>
+      <c r="G26">
+        <v>-0.183655</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>-0.203885</v>
+      </c>
+      <c r="B27">
+        <v>0.030279</v>
+      </c>
+      <c r="C27">
+        <v>237.14</v>
+      </c>
+      <c r="D27">
+        <v>-0.198543</v>
+      </c>
+      <c r="E27">
+        <v>0.005869</v>
+      </c>
+      <c r="F27">
+        <v>-0.170553</v>
+      </c>
+      <c r="G27">
+        <v>-0.184182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>-0.206104</v>
+      </c>
+      <c r="B28">
+        <v>0.030627</v>
+      </c>
+      <c r="C28">
+        <v>237.14</v>
+      </c>
+      <c r="D28">
+        <v>-0.200752</v>
+      </c>
+      <c r="E28">
+        <v>0.005851</v>
+      </c>
+      <c r="F28">
+        <v>-0.171405</v>
+      </c>
+      <c r="G28">
+        <v>-0.187075</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>-0.395179</v>
+      </c>
+      <c r="B29">
+        <v>4.402057</v>
+      </c>
+      <c r="C29">
+        <v>0.04</v>
+      </c>
+      <c r="D29">
+        <v>0.843373</v>
+      </c>
+      <c r="E29">
+        <v>0.061319</v>
+      </c>
+      <c r="F29">
+        <v>0.899333</v>
+      </c>
+      <c r="G29">
+        <v>0.9086109999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>-2.458495</v>
+      </c>
+      <c r="B30">
+        <v>10.727521</v>
+      </c>
+      <c r="C30">
+        <v>0.01</v>
+      </c>
+      <c r="D30">
+        <v>0.854729</v>
+      </c>
+      <c r="E30">
+        <v>0.054514</v>
+      </c>
+      <c r="F30">
+        <v>0.91361</v>
+      </c>
+      <c r="G30">
+        <v>0.913011</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>-6653.089754</v>
+      </c>
+      <c r="B31">
+        <v>45953.616341</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.881476</v>
+      </c>
+      <c r="E31">
+        <v>0.02569</v>
+      </c>
+      <c r="F31">
+        <v>0.8736120000000001</v>
+      </c>
+      <c r="G31">
+        <v>0.911717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>